<commit_message>
tutorial levels without popups lol
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut1.xlsx
+++ b/core/assets/levels/tut1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshyD\Documents\School\CS 3152 - Computer Game Architecture\MangoSnoopers\MangoSnoopers\core\assets\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E277A892-D30E-4BD5-A246-CD510F2794FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C57EC6-CCF2-4738-8A5B-5D6662944840}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="47">
   <si>
     <t>Region</t>
   </si>
@@ -72,10 +72,118 @@
     <t>File Name</t>
   </si>
   <si>
+    <t>TO ADD LATER: specify regions of the document and how many to select from each region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(∩ ͡° ͜ʖ ͡°)⊃━☆ﾟ. * ･ ｡ </t>
+  </si>
+  <si>
     <t>Key (Case Insensitive)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Region:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> The Burbs, Highway, Midwest, Colorado </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Speed:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Very slow, slow, normal, fast, very fast</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Song Genre:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Pop, Creepy, Dance, Action, Jazz, Thug, Comedy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Enemies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Gnome, Grill, Flamingo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Events:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Rear Enemy, Sun, Ned wakes up, Nosh wakes up, SAT Question</t>
+    </r>
+  </si>
+  <si>
     <t>END</t>
+  </si>
+  <si>
+    <r>
+      <t>Padding between enemies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Less, Normal, More</t>
+    </r>
   </si>
   <si>
     <t>Specifications</t>
@@ -84,7 +192,90 @@
     <t>Upload up to 5 songs and include the file extension. Song files should be stored in assets/RadioSongs</t>
   </si>
   <si>
+    <t>Each lane cell represents 50 in-game miles</t>
+  </si>
+  <si>
+    <t>To end the level, put "END" in the last row, in the events column</t>
+  </si>
+  <si>
+    <t>Padding between enemies defines how close together two rows will appear in-game.</t>
+  </si>
+  <si>
+    <t>If we make levels by shuffling random blocks:</t>
+  </si>
+  <si>
+    <t>Every block is (num lanes + 1) columns, beginning at column E.</t>
+  </si>
+  <si>
+    <t>For example, for a 3-lane highway, each block is 4 columns wide.</t>
+  </si>
+  <si>
     <t>To add a new block, copy the formatting of the block in the template beginning at the next column.</t>
+  </si>
+  <si>
+    <t>To end each block, still put "END" in the last row in the corresponding events column.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>total number of blocks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> field above should equal the total number of blocks you wrote in this doc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>number of blocks to use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> field above should equal the number of blocks you want to select from the</t>
+    </r>
+  </si>
+  <si>
+    <t>total number of blocks. For example, you could define 25 total blocks but want to randomly select</t>
+  </si>
+  <si>
+    <t>10 blocks to build the actual level in-game. Then, the total number of blocks field would be 25,</t>
+  </si>
+  <si>
+    <t>and the number of blocks to use would be 10.</t>
+  </si>
+  <si>
+    <t>Janky stuff we can change later:</t>
+  </si>
+  <si>
+    <t>Don't change number of lanes</t>
+  </si>
+  <si>
+    <t>Right now put 1 for total number of blocks and 1 for number of blocks to use</t>
   </si>
   <si>
     <t>Randomly select blocks</t>
@@ -99,183 +290,7 @@
     <t>Which blocks to use</t>
   </si>
   <si>
-    <t>** Don't change num lanes/random selection **</t>
-  </si>
-  <si>
-    <t>1, 2</t>
-  </si>
-  <si>
-    <t>Creepy</t>
-  </si>
-  <si>
-    <t>bensound-creepy.mp3</t>
-  </si>
-  <si>
-    <t>You can write any number of blocks. Pick which ones to use in the "which blocks to use" field</t>
-  </si>
-  <si>
-    <t>Block #s start from 1, list the ones you want separated by commas!!!!!!! : o )</t>
-  </si>
-  <si>
-    <t>(∩ ͡° ͜ʖ ͡°)⊃━☆ﾟ. * ･ ｡</t>
-  </si>
-  <si>
-    <r>
-      <t>Region:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>The Burbs, Highway, Midwest, Colorado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Speed:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Very slow, slow, normal, fast, very fast</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Song Genre:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pop, Creepy, Dance, Action, Jazz, Thug, Classical</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Enemies:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gnome, Grill start, grill end, Flamingo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Events:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Rear Enemy, Sun start, sun end, Ned wakes up, Nosh wakes up, SAT Question</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Padding between enemies: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Least (1.2), less (2.0), Normal (5.0), More (8.0), most (11.0), or a float not equal to 0.0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Roadside options:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Exit sign, Flamingo sale, A grill you can trust, Where will you be, The end is near</t>
-    </r>
-  </si>
-  <si>
-    <t>Padding between enemies defines how close together two rows will appear in-game (i.e. how many miles a cell represents)</t>
-  </si>
-  <si>
-    <t>To define multiple blocks:</t>
-  </si>
-  <si>
-    <t>Every block is (num lanes + 3) columns, beginning at column E.</t>
-  </si>
-  <si>
-    <t>For example, for a 3-lane highway, each block is 6 columns wide.</t>
-  </si>
-  <si>
-    <t>To end each block, put "END" in the last row in the corresponding events column.</t>
-  </si>
-  <si>
-    <t>You can define a level by stitching together certain blocks. Specify which blocks you want to use in the "which blocks to use"</t>
-  </si>
-  <si>
-    <t>field above. This should be a comma-separated list of the indices of blocks you want to use, where the first block is block 1.</t>
-  </si>
-  <si>
-    <t>Song options</t>
-  </si>
-  <si>
-    <t>bensound-countryboy.mp3</t>
-  </si>
-  <si>
-    <t>bensound-dance.mp3</t>
-  </si>
-  <si>
-    <t>bensound-extremeaction.mp3</t>
-  </si>
-  <si>
-    <t>bensound-funkyelement.mp3</t>
-  </si>
-  <si>
-    <t>bensound-jazzyfrenchy.mp3</t>
-  </si>
-  <si>
-    <t>bensound-ofeliasdream.mp3</t>
-  </si>
-  <si>
-    <t>rustling_leaves.mp3</t>
-  </si>
-  <si>
-    <t>testsong.mp3</t>
-  </si>
-  <si>
-    <t>testsong2.mp3</t>
-  </si>
-  <si>
-    <t>testsong3.mp3</t>
-  </si>
-  <si>
-    <t>Right Grass</t>
-  </si>
-  <si>
-    <t>Left Grass</t>
+    <t>Rear Enemy</t>
   </si>
 </sst>
 </file>
@@ -300,15 +315,33 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="'Calibri'"/>
     </font>
     <font>
+      <b/>
+      <u/>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="'Calibri'"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
     </font>
     <font>
       <u/>
@@ -324,35 +357,14 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF666666"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -361,8 +373,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -378,7 +389,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFE7E6E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -400,65 +411,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -743,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -784,24 +752,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>19</v>
+      <c r="D1" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>55</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
@@ -811,81 +777,61 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="22" t="s">
-        <v>56</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
+      <c r="D2" t="s">
+        <v>43</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
-        <v>23</v>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="G3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>45</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
+      <c r="C4" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
+      <c r="G4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A5">
+        <v>1</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
+      <c r="B5">
+        <v>1</v>
       </c>
-      <c r="B5" s="8">
-        <v>0.17</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="G5" s="11"/>
+      <c r="I5" s="11"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
@@ -893,366 +839,288 @@
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="2"/>
+      <c r="G6" s="11"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="G7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" customHeight="1">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="5" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A15" s="13" t="s">
-        <v>27</v>
+      <c r="A15" s="5" t="s">
+        <v>14</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="2" t="s">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="5" t="s">
+      <c r="I16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="G17" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="I17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A20" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="G18" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A21" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="2" t="s">
+      <c r="I18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A22" s="19" t="s">
-        <v>32</v>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="2" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="G19" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A23" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="5" t="s">
+      <c r="I19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A24" s="19" t="s">
-        <v>34</v>
+      <c r="A24" s="5" t="s">
+        <v>19</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A25" s="19" t="s">
-        <v>35</v>
+      <c r="A25" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="2" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A26" s="16" t="s">
-        <v>36</v>
+      <c r="A26" s="5" t="s">
+        <v>21</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="H27" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="G26" t="s">
         <v>9</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="1"/>
@@ -1261,62 +1129,84 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A28" s="15" t="s">
-        <v>16</v>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="G28" t="s">
+        <v>9</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="1" t="s">
-        <v>15</v>
+      <c r="I28" s="11" t="s">
+        <v>9</v>
       </c>
-      <c r="F28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A29" s="20" t="s">
-        <v>17</v>
+      <c r="A29" s="6" t="s">
+        <v>24</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A30" s="20" t="s">
-        <v>37</v>
+      <c r="A30" s="5" t="s">
+        <v>25</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="A31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:45" ht="16.899999999999999" customHeight="1">
-      <c r="A32" s="21" t="s">
-        <v>38</v>
+    <row r="32" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="I32" s="4"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1355,12 +1245,14 @@
       <c r="AS32" s="2"/>
     </row>
     <row r="33" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A33" s="20" t="s">
-        <v>39</v>
+      <c r="A33" s="5" t="s">
+        <v>28</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="12"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1399,12 +1291,18 @@
       <c r="AS33" s="2"/>
     </row>
     <row r="34" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A34" s="20" t="s">
-        <v>40</v>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" t="s">
+        <v>46</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="12"/>
+      <c r="G34" s="4"/>
+      <c r="H34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="4"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1443,12 +1341,14 @@
       <c r="AS34" s="2"/>
     </row>
     <row r="35" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A35" s="20" t="s">
-        <v>18</v>
+      <c r="A35" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="I35" s="4"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1487,12 +1387,14 @@
       <c r="AS35" s="2"/>
     </row>
     <row r="36" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A36" s="20" t="s">
-        <v>41</v>
+      <c r="A36" s="5" t="s">
+        <v>30</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="I36" s="4"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -1531,10 +1433,16 @@
       <c r="AS36" s="2"/>
     </row>
     <row r="37" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="A37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -1573,12 +1481,19 @@
       <c r="AS37" s="2"/>
     </row>
     <row r="38" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A38" s="17" t="s">
-        <v>42</v>
+      <c r="A38" s="5" t="s">
+        <v>32</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -1617,12 +1532,19 @@
       <c r="AS38" s="2"/>
     </row>
     <row r="39" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A39" s="17" t="s">
-        <v>43</v>
+      <c r="A39" s="5" t="s">
+        <v>33</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="G39" s="4"/>
+      <c r="H39" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1661,10 +1583,17 @@
       <c r="AS39" s="2"/>
     </row>
     <row r="40" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="G40" s="4"/>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1702,13 +1631,19 @@
       <c r="AR40" s="2"/>
       <c r="AS40" s="2"/>
     </row>
-    <row r="41" spans="1:45" ht="16.899999999999999" customHeight="1">
-      <c r="A41" s="21" t="s">
-        <v>44</v>
+    <row r="41" spans="1:45" ht="16.5" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>34</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="H41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -1747,12 +1682,21 @@
       <c r="AS41" s="2"/>
     </row>
     <row r="42" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A42" s="18" t="s">
-        <v>45</v>
+      <c r="A42" s="5" t="s">
+        <v>35</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="4"/>
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -1791,12 +1735,21 @@
       <c r="AS42" s="2"/>
     </row>
     <row r="43" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A43" s="18" t="s">
-        <v>26</v>
+      <c r="A43" s="5" t="s">
+        <v>36</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="4"/>
+      <c r="H43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -1835,12 +1788,21 @@
       <c r="AS43" s="2"/>
     </row>
     <row r="44" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A44" s="18" t="s">
-        <v>46</v>
+      <c r="A44" s="5" t="s">
+        <v>37</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="4"/>
+      <c r="H44" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -1879,12 +1841,21 @@
       <c r="AS44" s="2"/>
     </row>
     <row r="45" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A45" s="18" t="s">
-        <v>47</v>
+      <c r="A45" s="5" t="s">
+        <v>38</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="4"/>
+      <c r="H45" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -1923,12 +1894,19 @@
       <c r="AS45" s="2"/>
     </row>
     <row r="46" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A46" s="18" t="s">
-        <v>48</v>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="4"/>
+      <c r="H46" t="s">
+        <v>9</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -1967,12 +1945,21 @@
       <c r="AS46" s="2"/>
     </row>
     <row r="47" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A47" s="18" t="s">
-        <v>49</v>
+      <c r="A47" s="6" t="s">
+        <v>39</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="4"/>
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2011,12 +1998,21 @@
       <c r="AS47" s="2"/>
     </row>
     <row r="48" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A48" s="18" t="s">
-        <v>50</v>
+      <c r="A48" s="5" t="s">
+        <v>40</v>
       </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="4"/>
+      <c r="H48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2055,12 +2051,21 @@
       <c r="AS48" s="2"/>
     </row>
     <row r="49" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A49" s="18" t="s">
-        <v>51</v>
+      <c r="A49" s="5" t="s">
+        <v>41</v>
       </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="4"/>
+      <c r="H49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2099,12 +2104,19 @@
       <c r="AS49" s="2"/>
     </row>
     <row r="50" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A50" s="18" t="s">
-        <v>52</v>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" t="s">
+        <v>9</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -2143,12 +2155,19 @@
       <c r="AS50" s="2"/>
     </row>
     <row r="51" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A51" s="18" t="s">
-        <v>53</v>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3"/>
+      <c r="H51" t="s">
+        <v>9</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="I51" t="s">
+        <v>9</v>
+      </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -2187,12 +2206,19 @@
       <c r="AS51" s="2"/>
     </row>
     <row r="52" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A52" s="18" t="s">
-        <v>54</v>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="4"/>
+      <c r="H52" t="s">
+        <v>9</v>
       </c>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="I52" t="s">
+        <v>9</v>
+      </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -2231,15 +2257,19 @@
       <c r="AS52" s="2"/>
     </row>
     <row r="53" spans="1:45" ht="16.5" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="G53" s="4"/>
+      <c r="H53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
       <c r="J53" s="1"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -2284,9 +2314,13 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="G54" s="4"/>
+      <c r="H54" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" t="s">
+        <v>9</v>
+      </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -2331,9 +2365,13 @@
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
+      <c r="G55" s="4"/>
+      <c r="H55" t="s">
+        <v>9</v>
+      </c>
+      <c r="I55" t="s">
+        <v>9</v>
+      </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -2378,9 +2416,13 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
+      <c r="G56" s="4"/>
+      <c r="H56" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" t="s">
+        <v>9</v>
+      </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2423,11 +2465,15 @@
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="4"/>
+      <c r="H57" t="s">
+        <v>9</v>
+      </c>
+      <c r="I57" t="s">
+        <v>9</v>
+      </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -2472,9 +2518,13 @@
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
+      <c r="G58" s="4"/>
+      <c r="H58" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" t="s">
+        <v>9</v>
+      </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
@@ -2519,9 +2569,13 @@
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
+      <c r="G59" s="4"/>
+      <c r="H59" t="s">
+        <v>9</v>
+      </c>
+      <c r="I59" t="s">
+        <v>9</v>
+      </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -2566,9 +2620,13 @@
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="G60" s="4"/>
+      <c r="H60" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" t="s">
+        <v>9</v>
+      </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -2613,9 +2671,13 @@
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
+      <c r="G61" s="4"/>
+      <c r="H61" t="s">
+        <v>9</v>
+      </c>
+      <c r="I61" t="s">
+        <v>9</v>
+      </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
@@ -2660,9 +2722,13 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
+      <c r="G62" s="4"/>
+      <c r="H62" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" t="s">
+        <v>9</v>
+      </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -2708,8 +2774,12 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63" t="s">
+        <v>9</v>
+      </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
@@ -2752,11 +2822,13 @@
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -2802,8 +2874,8 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -2846,11 +2918,9 @@
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -2893,11 +2963,8 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -2940,11 +3007,8 @@
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
@@ -2990,8 +3054,8 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
@@ -3037,8 +3101,8 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -3084,8 +3148,8 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -3131,8 +3195,8 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
@@ -3363,8 +3427,8 @@
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -46787,25 +46851,7 @@
       <c r="AS1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:B23"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove print statement in radio
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut1.xlsx
+++ b/core/assets/levels/tut1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC4A648-AC25-4761-A4DC-7D518709CD26}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B889D6-C380-4884-98A9-151056FE8E0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9570" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
   <si>
     <t>Region</t>
   </si>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1049,9 +1049,6 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
       <c r="G23" s="4"/>
       <c r="H23" t="s">
         <v>9</v>
@@ -1067,6 +1064,9 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="G24" s="4"/>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="2"/>
     </row>
@@ -1101,8 +1101,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="G27" s="4"/>
-      <c r="H27" t="s">
+      <c r="G27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I27" t="s">
@@ -1118,8 +1117,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="G28" s="4"/>
-      <c r="H28" t="s">
+      <c r="G28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I28" t="s">
@@ -1137,10 +1135,10 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
       <c r="G29" s="4"/>
-      <c r="H29" t="s">
-        <v>9</v>
-      </c>
       <c r="I29" t="s">
         <v>9</v>
       </c>
@@ -1156,9 +1154,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="H30" t="s">
-        <v>9</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="I30" t="s">
         <v>9</v>
       </c>
@@ -1174,12 +1170,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
       <c r="G31" s="4"/>
-      <c r="H31" t="s">
-        <v>9</v>
-      </c>
       <c r="I31" t="s">
         <v>9</v>
       </c>
@@ -1195,12 +1186,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
       <c r="G32" s="4"/>
-      <c r="H32" t="s">
-        <v>9</v>
-      </c>
       <c r="I32" t="s">
         <v>9</v>
       </c>
@@ -1248,12 +1234,6 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="4"/>
-      <c r="H33" t="s">
-        <v>9</v>
-      </c>
       <c r="I33" t="s">
         <v>9</v>
       </c>
@@ -1405,8 +1385,8 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="4"/>
       <c r="H36" t="s">
         <v>9</v>
@@ -1564,9 +1544,9 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="4"/>
       <c r="H39" t="s">
         <v>9</v>
       </c>
@@ -1617,7 +1597,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
+      <c r="G40" s="4"/>
       <c r="H40" t="s">
         <v>9</v>
       </c>
@@ -1723,7 +1703,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="2"/>
       <c r="H42" t="s">
         <v>9</v>
       </c>
@@ -1776,7 +1756,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="3"/>
       <c r="H43" t="s">
         <v>9</v>
       </c>
@@ -1931,8 +1911,8 @@
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
       <c r="G46" s="4"/>
       <c r="H46" t="s">
         <v>9</v>
@@ -2090,8 +2070,8 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="4"/>
       <c r="H49" t="s">
         <v>9</v>
@@ -2245,7 +2225,7 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="G52" s="4"/>
       <c r="H52" t="s">
         <v>9</v>
       </c>
@@ -2294,13 +2274,15 @@
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="2" t="s">
-        <v>22</v>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="4"/>
+      <c r="H53" t="s">
+        <v>9</v>
       </c>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
       <c r="J53" s="1"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -2343,6 +2325,15 @@
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="4"/>
+      <c r="H54" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" t="s">
+        <v>9</v>
+      </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -2385,6 +2376,15 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" t="s">
+        <v>9</v>
+      </c>
+      <c r="I55" t="s">
+        <v>9</v>
+      </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -2427,6 +2427,13 @@
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>

</xml_diff>